<commit_message>
aded a way for password recovey
</commit_message>
<xml_diff>
--- a/database/members_info.xlsx
+++ b/database/members_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Python Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2CB728-8D23-4C22-B1EA-0FEC3FFA5947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B5231A-0C03-447D-AAE5-BD0054CA7937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4950" yWindow="4070" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>first name</t>
   </si>
@@ -31,6 +31,9 @@
     <t>phone number</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -43,56 +46,68 @@
     <t>date</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>Erfan</t>
   </si>
   <si>
     <t>Ghasemian</t>
   </si>
   <si>
+    <t>erfangh</t>
+  </si>
+  <si>
+    <t>Erfan@gmail.com</t>
+  </si>
+  <si>
+    <t>Erfan@123</t>
+  </si>
+  <si>
+    <t>Tehran</t>
+  </si>
+  <si>
+    <t>2005/January/1</t>
+  </si>
+  <si>
+    <t>Arian</t>
+  </si>
+  <si>
+    <t>Saedkondori</t>
+  </si>
+  <si>
+    <t>ariansk</t>
+  </si>
+  <si>
+    <t>Arian@yahoo.com</t>
+  </si>
+  <si>
+    <t>Arian@123</t>
+  </si>
+  <si>
+    <t>Karaj</t>
+  </si>
+  <si>
+    <t>ghasemian</t>
+  </si>
+  <si>
+    <t>erfanGh</t>
+  </si>
+  <si>
+    <t>erfan</t>
+  </si>
+  <si>
     <t>09112868820</t>
   </si>
   <si>
-    <t>Erfan@gmail.com</t>
-  </si>
-  <si>
-    <t>Erfan@123</t>
-  </si>
-  <si>
-    <t>Tehran</t>
-  </si>
-  <si>
-    <t>2005/January/1</t>
-  </si>
-  <si>
-    <t>erfangh</t>
-  </si>
-  <si>
-    <t>Arian</t>
-  </si>
-  <si>
-    <t>Saedkondori</t>
-  </si>
-  <si>
-    <t>ariansk</t>
-  </si>
-  <si>
-    <t>Arian@yahoo.com</t>
-  </si>
-  <si>
-    <t>Arian@123</t>
-  </si>
-  <si>
-    <t>Karaj</t>
+    <t>erfanGH</t>
+  </si>
+  <si>
+    <t>erfan@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,14 +119,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,19 +153,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,20 +463,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -486,19 +490,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -508,11 +512,11 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>9112868820</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -529,35 +533,83 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
       <c r="C3">
         <v>9125623357</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>9112868820</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{79DD470B-5F01-475D-8C47-8A4E242FB301}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{63ECAA28-2120-41B6-A290-0C1FB7149A68}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made login and sign up 10X better
</commit_message>
<xml_diff>
--- a/database/members_info.xlsx
+++ b/database/members_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,88 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>9112868830</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>erfangg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Erfan@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Erfan@123</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Tehran</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2005/February/26</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Erfan</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ghasemian</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>09112868820</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>erfangh</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>erfan.ghasemian40@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Erfan@123</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Tehran</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2005/January/1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
filter section + bug fix
</commit_message>
<xml_diff>
--- a/database/members_info.xlsx
+++ b/database/members_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,34 +474,46 @@
           <t>date</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>security type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>security answer</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>Erfan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>9112868830</v>
+          <t>Ghasemian</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>09112868820</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>erfangg</t>
+          <t>erfangh</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Erfan@gmail.com</t>
+          <t>erfan.ghasemian40@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Erfan@123</t>
+          <t>Erfan@12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -511,49 +523,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2005/February/26</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Erfan</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ghasemian</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>09112868820</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>erfangh</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>erfan.ghasemian40@gmail.com</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Erfan@123</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tehran</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t>2005/January/1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Babol</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished main window and bug fixes
</commit_message>
<xml_diff>
--- a/database/members_info.xlsx
+++ b/database/members_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,10 +496,8 @@
           <t>Ghasemian</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>09112868820</t>
-        </is>
+      <c r="C2" t="n">
+        <v>9112868820</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -534,6 +532,58 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>Babol</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Arian</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Saeedkondori</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>09112868830</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ariansk</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>arian@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Arian@12</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Karaj</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2005/January/1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Karaj</t>
         </is>
       </c>
     </row>

</xml_diff>